<commit_message>
Analyte list cleanup implemented
</commit_message>
<xml_diff>
--- a/Target_List_Demo.xlsx
+++ b/Target_List_Demo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josephmonaghan/Documents/nanoDESI_raw_to_imzml/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F5873A2-E6F8-2946-87B5-048E28181517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F50570-AE9F-074A-9845-3301FF87C691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{1D3F4346-8B06-9947-A01A-C95E4397CEDD}"/>
   </bookViews>
@@ -443,7 +443,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>